<commit_message>
HTML GRAPH Part4 - Inprogress
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/LIVE_INTERVIEW_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/LIVE_INTERVIEW_HISTORY_DATA.xlsx
@@ -19,8 +19,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -65,12 +65,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -436,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,8 +488,8 @@
           <t>2021-06-04</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>44351.46543855745</v>
+      <c r="B2" s="3" t="n">
+        <v>44351.46543855324</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -508,6 +509,64 @@
       </c>
       <c r="G2" t="n">
         <v>2.912727216666667</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-06-07</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>44354.77812368055</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>regression_145final</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>103</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3.699947816666667</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021-06-08</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>44355.52055797454</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>regression_final_145</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>101</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.896933683333333</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,6 +623,35 @@
         <is>
           <t>Time Taken</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2021-06-08</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>44355.6871661205</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>145_beta</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4.358921433333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTML REPORT GENERATOR - PART3
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/LIVE_INTERVIEW_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/LIVE_INTERVIEW_HISTORY_DATA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="AMSIN" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,8 +19,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="164"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -63,20 +63,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -570,7 +570,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -580,7 +580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>44355.6871661205</v>
+        <v>44355.68716612268</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -654,8 +654,37 @@
         <v>4.358921433333333</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-06-09</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>44356.6332471106</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>145_beta</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.857780133333333</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -711,7 +740,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -767,6 +796,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>